<commit_message>
Cleaned and Commented Descriptions Module. Working version of Setup.py
</commit_message>
<xml_diff>
--- a/data/Input_phase_List.xlsx
+++ b/data/Input_phase_List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yaseen.Ali\OneDrive - Callisto Integration\Documents\Python Scripts and Training\My Projects\Archestra_Desc_Generator\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yaseen.Ali\OneDrive - Callisto Integration\Documents\Python Scripts and Training\Archestra_Desc_Generator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
     <t>_121070060UN_MLP_LINE_26</t>
   </si>
   <si>
-    <t>FM_PHS001_Refill_MLP_Line_26_Hopper</t>
+    <t>FM_PHS002_Run_MLP26_to_Storeveyor</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -406,6 +406,9 @@
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -413,12 +416,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B29137B0964ABD49853DF67CD151539D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="40d80cd8488f5694a276c11424603e2e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="af46c936-2cfc-491e-b590-64fbb9c74407" xmlns:ns4="8d5d32e6-4160-4ea1-b873-fac29d433bfc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8c18cd32d045ae290bebe310ac348b65" ns3:_="" ns4:_="">
     <xsd:import namespace="af46c936-2cfc-491e-b590-64fbb9c74407"/>
@@ -635,6 +632,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -645,23 +648,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95C557E6-0EF9-4EFF-983A-E1D8BB7EC6BE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="af46c936-2cfc-491e-b590-64fbb9c74407"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8d5d32e6-4160-4ea1-b873-fac29d433bfc"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DC0AECB-23C1-46A3-A457-994C9B7192FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -680,6 +666,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95C557E6-0EF9-4EFF-983A-E1D8BB7EC6BE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="af46c936-2cfc-491e-b590-64fbb9c74407"/>
+    <ds:schemaRef ds:uri="8d5d32e6-4160-4ea1-b873-fac29d433bfc"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F72D078E-E017-4C6A-8772-BD816321B60C}">
   <ds:schemaRefs>

</xml_diff>